<commit_message>
Final push, whole project and outputs
</commit_message>
<xml_diff>
--- a/Project Outputs for JouleScopeBoard/BOM/Bill of Materials-JouleScopeBoard.xlsx
+++ b/Project Outputs for JouleScopeBoard/BOM/Bill of Materials-JouleScopeBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Work\Design\JouleScopeBoard\Project Outputs for JouleScopeBoard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A635D0CE-4151-469A-BBF1-D68CECB36052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E304CE8A-CD0C-4545-8B20-CEEBEBE1267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="25740" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -142,10 +142,10 @@
     <t>&lt;Parameter ClientContactEmail not found&gt;</t>
   </si>
   <si>
-    <t>17/10/2023</t>
-  </si>
-  <si>
-    <t>14:33</t>
+    <t>23/10/2023</t>
+  </si>
+  <si>
+    <t>15:17</t>
   </si>
   <si>
     <t>&lt;Parameter ClientWebsite not found&gt;</t>
@@ -223,10 +223,10 @@
     <t>C:\Temp\Work\Design\JouleScopeBoard\JouleScopeBoard.PrjPcb</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>17/10/2023 14:33</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>23/10/2023 15:17</t>
   </si>
   <si>
     <t>Bill of Materials</t>
@@ -1619,27 +1619,27 @@
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="31" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="76" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="76" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.26953125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" style="1"/>
+    <col min="15" max="15" width="8.28515625" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52"/>
       <c r="B1" s="53"/>
       <c r="C1" s="54"/>
@@ -1656,7 +1656,7 @@
       <c r="N1" s="53"/>
       <c r="O1" s="62"/>
     </row>
-    <row r="2" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="s">
@@ -1676,7 +1676,7 @@
       <c r="N2" s="12"/>
       <c r="O2" s="63"/>
     </row>
-    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -1697,7 +1697,7 @@
       <c r="M3" s="2"/>
       <c r="O3" s="64"/>
     </row>
-    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="55"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
@@ -1715,7 +1715,7 @@
       <c r="J4" s="15"/>
       <c r="O4" s="64"/>
     </row>
-    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="55"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="O5" s="64"/>
     </row>
-    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="55"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -1752,7 +1752,7 @@
       <c r="K6" s="13"/>
       <c r="O6" s="64"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="55"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20" t="s">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="O7" s="64"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="55"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
@@ -1783,11 +1783,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>45216</v>
+        <v>45222</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>45216.606641666665</v>
+        <v>45222.637350115743</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -1796,7 +1796,7 @@
       <c r="K8" s="15"/>
       <c r="O8" s="64"/>
     </row>
-    <row r="9" spans="1:15" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="35" t="s">
         <v>22</v>
@@ -1841,7 +1841,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="55"/>
       <c r="B10" s="29">
         <f>ROW(B10) - ROW($B$9)</f>
@@ -1869,7 +1869,7 @@
       <c r="N10" s="81"/>
       <c r="O10" s="65"/>
     </row>
-    <row r="11" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="55"/>
       <c r="B11" s="31">
         <f>ROW(B11) - ROW($B$9)</f>
@@ -1897,7 +1897,7 @@
       <c r="N11" s="82"/>
       <c r="O11" s="66"/>
     </row>
-    <row r="12" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="55"/>
       <c r="B12" s="29">
         <f>ROW(B12) - ROW($B$9)</f>
@@ -1915,7 +1915,7 @@
         <v>52</v>
       </c>
       <c r="H12" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="74"/>
       <c r="J12" s="30"/>
@@ -1925,7 +1925,7 @@
       <c r="N12" s="81"/>
       <c r="O12" s="65"/>
     </row>
-    <row r="13" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="31">
         <f>ROW(B13) - ROW($B$9)</f>
@@ -1943,7 +1943,7 @@
         <v>53</v>
       </c>
       <c r="H13" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="75"/>
       <c r="J13" s="32"/>
@@ -1953,7 +1953,7 @@
       <c r="N13" s="82"/>
       <c r="O13" s="66"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="55"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50"/>
@@ -1962,7 +1962,7 @@
       <c r="F14" s="47"/>
       <c r="H14" s="46">
         <f>SUM(H10:H13)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="46">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="O14" s="67"/>
     </row>
-    <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
       <c r="B15" s="83" t="s">
         <v>20</v>
@@ -1993,7 +1993,7 @@
       <c r="I15" s="77"/>
       <c r="O15" s="64"/>
     </row>
-    <row r="16" spans="1:15" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="55"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="O16" s="64"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="55"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="O17" s="64"/>
     </row>
-    <row r="18" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57"/>
       <c r="B18" s="27"/>
       <c r="C18" s="11"/>
@@ -2061,17 +2061,17 @@
       <c r="N18" s="58"/>
       <c r="O18" s="68"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2115,13 +2115,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.54296875" customWidth="1"/>
+    <col min="2" max="2" width="110.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>

</xml_diff>